<commit_message>
unit tests added and README.md completed
</commit_message>
<xml_diff>
--- a/tests/data/testdata.xlsx
+++ b/tests/data/testdata.xlsx
@@ -401,7 +401,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,10 +467,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>

</xml_diff>